<commit_message>
Tales Colab 2 GLO + JAP
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12285" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12285" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="캐릭터" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="특성번역" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'캐릭터'!$A$1:$Q$294</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'캐릭터'!$A$1:$Q$299</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'보너스'!$A$1:$D$87</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -27,7 +27,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -70,6 +70,22 @@
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="128"/>
+      <family val="3"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -475,11 +491,11 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q294"/>
+  <dimension ref="A1:Q303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P201" sqref="P201"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D296" sqref="D296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -6545,7 +6561,7 @@
       </c>
       <c r="Q113" s="1" t="inlineStr">
         <is>
-          <t>현현</t>
+          <t>진현현</t>
         </is>
       </c>
     </row>
@@ -8653,7 +8669,7 @@
       </c>
       <c r="L152" s="2" t="inlineStr">
         <is>
-          <t>152,153</t>
+          <t>152,153,294</t>
         </is>
       </c>
     </row>
@@ -8701,8 +8717,10 @@
       <c r="K153" s="2" t="n">
         <v>151</v>
       </c>
-      <c r="L153" s="2" t="n">
-        <v>153</v>
+      <c r="L153" s="2" t="inlineStr">
+        <is>
+          <t>153,294</t>
+        </is>
       </c>
       <c r="M153" s="1" t="inlineStr">
         <is>
@@ -15954,8 +15972,451 @@
         </is>
       </c>
     </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B295" s="1" t="inlineStr">
+        <is>
+          <t>월화의 영애 히스메나</t>
+        </is>
+      </c>
+      <c r="C295" s="1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="D295" s="2" t="inlineStr">
+        <is>
+          <t>101010141</t>
+        </is>
+      </c>
+      <c r="E295" s="1" t="inlineStr">
+        <is>
+          <t>물</t>
+        </is>
+      </c>
+      <c r="F295" s="1" t="inlineStr">
+        <is>
+          <t>검</t>
+        </is>
+      </c>
+      <c r="G295" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H295" s="1" t="inlineStr">
+        <is>
+          <t>명</t>
+        </is>
+      </c>
+      <c r="I295" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J295" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L295" s="2" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="M295" s="1" t="inlineStr">
+        <is>
+          <t>프로일라인</t>
+        </is>
+      </c>
+      <c r="N295" s="1" t="inlineStr">
+        <is>
+          <t>경전록</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B296" s="1" t="inlineStr">
+        <is>
+          <t>로이드</t>
+        </is>
+      </c>
+      <c r="C296" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D296" s="2" t="inlineStr">
+        <is>
+          <t>101450011</t>
+        </is>
+      </c>
+      <c r="E296" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F296" s="1" t="inlineStr">
+        <is>
+          <t>도</t>
+        </is>
+      </c>
+      <c r="G296" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H296" s="1" t="inlineStr">
+        <is>
+          <t>천</t>
+        </is>
+      </c>
+      <c r="I296" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J296" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L296" s="2" t="inlineStr">
+        <is>
+          <t>296</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B297" s="1" t="inlineStr">
+        <is>
+          <t>로이드</t>
+        </is>
+      </c>
+      <c r="C297" s="1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="D297" s="2" t="inlineStr">
+        <is>
+          <t>101450011</t>
+        </is>
+      </c>
+      <c r="E297" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F297" s="1" t="inlineStr">
+        <is>
+          <t>도</t>
+        </is>
+      </c>
+      <c r="G297" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H297" s="1" t="inlineStr">
+        <is>
+          <t>천</t>
+        </is>
+      </c>
+      <c r="I297" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J297" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K297" s="2" t="inlineStr">
+        <is>
+          <t>295</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B298" s="1" t="inlineStr">
+        <is>
+          <t>콜레트</t>
+        </is>
+      </c>
+      <c r="C298" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D298" s="2" t="inlineStr">
+        <is>
+          <t>101450021</t>
+        </is>
+      </c>
+      <c r="E298" s="1" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="F298" s="1" t="inlineStr">
+        <is>
+          <t>지팡이</t>
+        </is>
+      </c>
+      <c r="G298" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H298" s="1" t="inlineStr">
+        <is>
+          <t>천</t>
+        </is>
+      </c>
+      <c r="I298" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J298" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L298" s="2" t="inlineStr">
+        <is>
+          <t>298</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B299" s="1" t="inlineStr">
+        <is>
+          <t>콜레트</t>
+        </is>
+      </c>
+      <c r="C299" s="1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="D299" s="2" t="inlineStr">
+        <is>
+          <t>101450021</t>
+        </is>
+      </c>
+      <c r="E299" s="1" t="inlineStr">
+        <is>
+          <t>기타</t>
+        </is>
+      </c>
+      <c r="F299" s="1" t="inlineStr">
+        <is>
+          <t>지팡이</t>
+        </is>
+      </c>
+      <c r="G299" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H299" s="1" t="inlineStr">
+        <is>
+          <t>천</t>
+        </is>
+      </c>
+      <c r="I299" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J299" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K299" s="2" t="inlineStr">
+        <is>
+          <t>297</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B300" s="1" t="inlineStr">
+        <is>
+          <t>알펜</t>
+        </is>
+      </c>
+      <c r="C300" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D300" s="2" t="inlineStr">
+        <is>
+          <t>101450031</t>
+        </is>
+      </c>
+      <c r="E300" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F300" s="1" t="inlineStr">
+        <is>
+          <t>검</t>
+        </is>
+      </c>
+      <c r="G300" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H300" s="1" t="inlineStr">
+        <is>
+          <t>명</t>
+        </is>
+      </c>
+      <c r="I300" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J300" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L300" s="2" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B301" s="1" t="inlineStr">
+        <is>
+          <t>알펜</t>
+        </is>
+      </c>
+      <c r="C301" s="1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="D301" s="2" t="inlineStr">
+        <is>
+          <t>101450031</t>
+        </is>
+      </c>
+      <c r="E301" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F301" s="1" t="inlineStr">
+        <is>
+          <t>검</t>
+        </is>
+      </c>
+      <c r="G301" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H301" s="1" t="inlineStr">
+        <is>
+          <t>명</t>
+        </is>
+      </c>
+      <c r="I301" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J301" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K301" s="2" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B302" s="1" t="inlineStr">
+        <is>
+          <t>시온 (테일즈)</t>
+        </is>
+      </c>
+      <c r="C302" s="1" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D302" s="2" t="inlineStr">
+        <is>
+          <t>101450041</t>
+        </is>
+      </c>
+      <c r="E302" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F302" s="1" t="inlineStr">
+        <is>
+          <t>활</t>
+        </is>
+      </c>
+      <c r="G302" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H302" s="1" t="inlineStr">
+        <is>
+          <t>명</t>
+        </is>
+      </c>
+      <c r="I302" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J302" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L302" s="2" t="inlineStr">
+        <is>
+          <t>302</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B303" s="1" t="inlineStr">
+        <is>
+          <t>시온 (테일즈)</t>
+        </is>
+      </c>
+      <c r="C303" s="1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="D303" s="2" t="inlineStr">
+        <is>
+          <t>101450041</t>
+        </is>
+      </c>
+      <c r="E303" s="1" t="inlineStr">
+        <is>
+          <t>불</t>
+        </is>
+      </c>
+      <c r="F303" s="1" t="inlineStr">
+        <is>
+          <t>활</t>
+        </is>
+      </c>
+      <c r="G303" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H303" s="1" t="inlineStr">
+        <is>
+          <t>명</t>
+        </is>
+      </c>
+      <c r="I303" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J303" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K303" s="2" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q294"/>
+  <autoFilter ref="A1:Q299"/>
   <hyperlinks>
     <hyperlink ref="D270" tooltip="File:101000301 rank5 command.png" display="https://anothereden.miraheze.org/wiki/File:101000301_rank5_command.png" r:id="rId1"/>
   </hyperlinks>
@@ -16157,10 +16618,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -16170,8 +16631,8 @@
     <col width="25" customWidth="1" style="1" min="4" max="4"/>
     <col width="25" customWidth="1" style="2" min="5" max="5"/>
     <col width="25" customWidth="1" style="1" min="6" max="19"/>
-    <col width="9" customWidth="1" style="1" min="20" max="35"/>
-    <col width="9" customWidth="1" style="1" min="36" max="16384"/>
+    <col width="9" customWidth="1" style="1" min="20" max="37"/>
+    <col width="9" customWidth="1" style="1" min="38" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -19149,6 +19610,106 @@
       <c r="E159" s="2" t="inlineStr">
         <is>
           <t>101060161</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>월화의 영애 히스메나</t>
+        </is>
+      </c>
+      <c r="B160" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C160" s="1" t="inlineStr">
+        <is>
+          <t>검,IDA스쿨</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="inlineStr">
+        <is>
+          <t>101010141</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
+        <is>
+          <t>로이드</t>
+        </is>
+      </c>
+      <c r="B161" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C161" s="1" t="inlineStr">
+        <is>
+          <t>도</t>
+        </is>
+      </c>
+      <c r="E161" s="2" t="inlineStr">
+        <is>
+          <t>101450011</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>콜레트</t>
+        </is>
+      </c>
+      <c r="B162" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C162" s="1" t="inlineStr">
+        <is>
+          <t>지팡이</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="inlineStr">
+        <is>
+          <t>101450021</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
+        <is>
+          <t>알펜</t>
+        </is>
+      </c>
+      <c r="B163" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C163" s="1" t="inlineStr">
+        <is>
+          <t>가면,검,기억상실</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="inlineStr">
+        <is>
+          <t>101450031</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>시온 (테일즈)</t>
+        </is>
+      </c>
+      <c r="B164" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C164" s="1" t="inlineStr">
+        <is>
+          <t>활,대식가,총</t>
+        </is>
+      </c>
+      <c r="E164" s="2" t="inlineStr">
+        <is>
+          <t>101450041</t>
         </is>
       </c>
     </row>
@@ -19169,7 +19730,7 @@
   </sheetPr>
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
@@ -22495,7 +23056,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -23178,10 +23739,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C308"/>
+  <dimension ref="A1:C314"/>
   <sheetViews>
-    <sheetView topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="C308" sqref="C308"/>
+    <sheetView topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -28425,9 +28986,113 @@
         </is>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" s="1" t="inlineStr">
+        <is>
+          <t>프로일라인</t>
+        </is>
+      </c>
+      <c r="B309" s="1" t="inlineStr">
+        <is>
+          <t>Fraulein</t>
+        </is>
+      </c>
+      <c r="C309" s="1" t="inlineStr">
+        <is>
+          <t>フロイライン</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="inlineStr">
+        <is>
+          <t>월화의 영애 히스메나</t>
+        </is>
+      </c>
+      <c r="B310" s="1" t="inlineStr">
+        <is>
+          <t>Hismena (Alter)</t>
+        </is>
+      </c>
+      <c r="C310" s="1" t="inlineStr">
+        <is>
+          <t>月華の令嬢 ヒスメナ</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
+          <t>로이드</t>
+        </is>
+      </c>
+      <c r="B311" s="1" t="inlineStr">
+        <is>
+          <t>Lloyd</t>
+        </is>
+      </c>
+      <c r="C311" s="1" t="inlineStr">
+        <is>
+          <t>ロイド</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="inlineStr">
+        <is>
+          <t>콜레트</t>
+        </is>
+      </c>
+      <c r="B312" s="1" t="inlineStr">
+        <is>
+          <t>Colette</t>
+        </is>
+      </c>
+      <c r="C312" s="1" t="inlineStr">
+        <is>
+          <t>コレット</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="inlineStr">
+        <is>
+          <t>알펜</t>
+        </is>
+      </c>
+      <c r="B313" s="1" t="inlineStr">
+        <is>
+          <t>Alphen</t>
+        </is>
+      </c>
+      <c r="C313" s="1" t="inlineStr">
+        <is>
+          <t>アルフェン</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="inlineStr">
+        <is>
+          <t>시온 (테일즈)</t>
+        </is>
+      </c>
+      <c r="B314" s="1" t="inlineStr">
+        <is>
+          <t>Shionne (Tales)</t>
+        </is>
+      </c>
+      <c r="C314" s="1" t="inlineStr">
+        <is>
+          <t>シオン (テイルズ)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B282" tooltip="Shion (Alter)" display="https://anothereden.miraheze.org/wiki/Shion_(Alter)" r:id="rId1"/>
+    <hyperlink ref="C313" display="https://altema.jp/anaden/chara/984" r:id="rId2"/>
+    <hyperlink ref="C314" display="https://altema.jp/anaden/chara/985" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>